<commit_message>
update ip and ... xlsx
</commit_message>
<xml_diff>
--- a/@@KBRO PM_Template_20210512.xlsx
+++ b/@@KBRO PM_Template_20210512.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="20520" windowHeight="4260"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="20520" windowHeight="4260" tabRatio="910"/>
   </bookViews>
   <sheets>
     <sheet name="IP" sheetId="1" r:id="rId1"/>
@@ -14,18 +14,20 @@
     <sheet name="DTI" sheetId="9" r:id="rId5"/>
     <sheet name="CGNAT" sheetId="23" r:id="rId6"/>
     <sheet name="QB" sheetId="15" r:id="rId7"/>
-    <sheet name="使用說明" sheetId="18" r:id="rId8"/>
-    <sheet name="功能" sheetId="19" r:id="rId9"/>
-    <sheet name="ASR IP " sheetId="17" r:id="rId10"/>
+    <sheet name="ASR IP " sheetId="17" r:id="rId8"/>
+    <sheet name="QB IP" sheetId="25" r:id="rId9"/>
+    <sheet name="CGNAT IP" sheetId="24" r:id="rId10"/>
     <sheet name="CMTS IP" sheetId="21" r:id="rId11"/>
     <sheet name="中區IP" sheetId="22" r:id="rId12"/>
+    <sheet name="功能" sheetId="19" r:id="rId13"/>
+    <sheet name="使用說明" sheetId="18" r:id="rId14"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="430">
   <si>
     <t>IP</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2380,12 +2382,391 @@
     <t>shell cat /flash/nsconfig/ZebOS.conf</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>&lt;&lt;有預設的帳密</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CGNAT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>鳳信</t>
+    </r>
+  </si>
+  <si>
+    <t>PHC_CGNAT1</t>
+  </si>
+  <si>
+    <t>192.168.169.24</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>觀昇</t>
+    </r>
+  </si>
+  <si>
+    <t>KS_CGNAT1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.222.104.24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>南天</t>
+    </r>
+  </si>
+  <si>
+    <t>NT_CGNAT1</t>
+  </si>
+  <si>
+    <t>10.220.96.24</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>新頻道</t>
+    </r>
+  </si>
+  <si>
+    <t>NCC_CGNAT1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.222.88.24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>豐盟</t>
+    </r>
+  </si>
+  <si>
+    <t>FM_CGNAT1</t>
+  </si>
+  <si>
+    <t>10.222.80.24</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>永佳樂</t>
+    </r>
+  </si>
+  <si>
+    <t>YJL_CGNAT1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>金頻道</t>
+    </r>
+  </si>
+  <si>
+    <t>KP_CGNAT1</t>
+  </si>
+  <si>
+    <t>10.222.32.24</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>聯禾</t>
+    </r>
+  </si>
+  <si>
+    <t>UCT_CGNAT1</t>
+  </si>
+  <si>
+    <t>192.168.160.40</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>北桃園</t>
+    </r>
+  </si>
+  <si>
+    <t>BNT_CGNAT1</t>
+  </si>
+  <si>
+    <t>10.222.64.24</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="細明體"/>
+        <family val="3"/>
+        <charset val="136"/>
+      </rPr>
+      <t>全聯</t>
+    </r>
+  </si>
+  <si>
+    <t>UC_CGNAT1</t>
+  </si>
+  <si>
+    <t>10.222.56.24</t>
+  </si>
+  <si>
+    <t>DEVICE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HOST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鳳信</t>
+  </si>
+  <si>
+    <t>PHC_QB200</t>
+  </si>
+  <si>
+    <t>192.168.169.1,192.168.169.2</t>
+  </si>
+  <si>
+    <t>紅樹林</t>
+  </si>
+  <si>
+    <t>MCT_QB200</t>
+  </si>
+  <si>
+    <t>192.168.144.38,192.168.144.39</t>
+  </si>
+  <si>
+    <t>觀天下</t>
+  </si>
+  <si>
+    <t>GVC_QB200</t>
+  </si>
+  <si>
+    <t>192.168.152.38,192.168.152.39</t>
+  </si>
+  <si>
+    <t>聯禾有線電視</t>
+  </si>
+  <si>
+    <t>UCT_QB200</t>
+  </si>
+  <si>
+    <t>192.168.160.28,192.168.160.29</t>
+  </si>
+  <si>
+    <t>YJL_QB200</t>
+  </si>
+  <si>
+    <t>192.168.136.19,192.168.136.20</t>
+  </si>
+  <si>
+    <t>觀昇</t>
+  </si>
+  <si>
+    <t>LGS_QB200</t>
+  </si>
+  <si>
+    <t>10.222.104.236,10.222.104.237</t>
+  </si>
+  <si>
+    <t>南天</t>
+  </si>
+  <si>
+    <t>JNT_QB200</t>
+  </si>
+  <si>
+    <t>10.220.96.236,10.220.96.237</t>
+  </si>
+  <si>
+    <t>新頻道</t>
+  </si>
+  <si>
+    <t>FNC_QB200</t>
+  </si>
+  <si>
+    <t>豐盟</t>
+  </si>
+  <si>
+    <t>EFM_QB200</t>
+  </si>
+  <si>
+    <t>10.222.80.236,10.222.80.237</t>
+  </si>
+  <si>
+    <t>振道有線電視</t>
+  </si>
+  <si>
+    <t>CHC_QB200</t>
+  </si>
+  <si>
+    <t>10.222.72.236,10.222.72.237</t>
+  </si>
+  <si>
+    <t>文山</t>
+  </si>
+  <si>
+    <t>AWS_QB200</t>
+  </si>
+  <si>
+    <t>10.222.44.236,10.222.44.237</t>
+  </si>
+  <si>
+    <t>大安</t>
+  </si>
+  <si>
+    <t>ATA_QB200</t>
+  </si>
+  <si>
+    <t>10.222.40.236,10.222.40.237</t>
+  </si>
+  <si>
+    <t>ACL_QB200</t>
+  </si>
+  <si>
+    <t>10.222.56.236,10.222.56.237</t>
+  </si>
+  <si>
+    <t>陽明山</t>
+  </si>
+  <si>
+    <t>AYM_QB200</t>
+  </si>
+  <si>
+    <t>10.222.16.236,10.222.16.237</t>
+  </si>
+  <si>
+    <t>北桃園有線電視</t>
+  </si>
+  <si>
+    <t>BTN_QB200</t>
+  </si>
+  <si>
+    <t>10.222.64.236,10.222.64.237</t>
+  </si>
+  <si>
+    <t>金頻道</t>
+  </si>
+  <si>
+    <t>AGC_QB200</t>
+  </si>
+  <si>
+    <t>10.222.32.236,10.222.32.237</t>
+  </si>
+  <si>
+    <t>CG有線電視</t>
+  </si>
+  <si>
+    <t>ACG_QB200</t>
+  </si>
+  <si>
+    <t>10.222.112.236,10.222.112.237</t>
+  </si>
+  <si>
+    <t>新唐城</t>
+  </si>
+  <si>
+    <t>ANC_QB200</t>
+  </si>
+  <si>
+    <t>10.222.48.236,10.222.48.237</t>
+  </si>
+  <si>
+    <t>新台北</t>
+  </si>
+  <si>
+    <t>ANT_QB200</t>
+  </si>
+  <si>
+    <t>10.222.24.236,10.222.24.237</t>
+  </si>
+  <si>
+    <t>DEVICE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HOST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2524,7 +2905,7 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2543,8 +2924,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -2552,27 +2939,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2669,7 +3041,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2678,17 +3049,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2698,6 +3062,16 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2719,6 +3093,239 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>8443688</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>46119</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="圖片 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="45720" y="419100"/>
+          <a:ext cx="8397968" cy="4595259"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6751900</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>129945</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="圖片 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="60960" y="5570220"/>
+          <a:ext cx="6690940" cy="4671465"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6660450</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>91740</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="圖片 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="83820" y="10904220"/>
+          <a:ext cx="6576630" cy="3459780"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>6530898</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>15533</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="圖片 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="91440" y="14607540"/>
+          <a:ext cx="6439458" cy="3383573"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>153172</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>152551</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="圖片 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="18051780"/>
+          <a:ext cx="8900932" cy="1737511"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>7544448</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>61224</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="圖片 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="20025360"/>
+          <a:ext cx="7468248" cy="3040644"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3101,239 +3708,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>8443688</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>46119</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="圖片 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="45720" y="419100"/>
-          <a:ext cx="8397968" cy="4595259"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>6751900</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>129945</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="圖片 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="60960" y="5570220"/>
-          <a:ext cx="6690940" cy="4671465"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>6660450</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>91740</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="圖片 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="83820" y="10904220"/>
-          <a:ext cx="6576630" cy="3459780"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>6530898</xdr:colOff>
-      <xdr:row>89</xdr:row>
-      <xdr:rowOff>15533</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="圖片 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="91440" y="14607540"/>
-          <a:ext cx="6439458" cy="3383573"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>153172</xdr:colOff>
-      <xdr:row>101</xdr:row>
-      <xdr:rowOff>152551</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="圖片 6"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="18051780"/>
-          <a:ext cx="8900932" cy="1737511"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>102</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>7544448</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>61224</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="圖片 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="76200" y="20025360"/>
-          <a:ext cx="7468248" cy="3040644"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
@@ -3624,26 +3998,27 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" style="42" customWidth="1"/>
+    <col min="1" max="1" width="28.21875" style="41" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.109375" style="35" customWidth="1"/>
     <col min="3" max="3" width="14.21875" style="35" customWidth="1"/>
     <col min="4" max="4" width="8.44140625" style="35" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="3"/>
+    <col min="7" max="7" width="17.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:7" ht="16.2">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="33" t="s">
@@ -3655,426 +4030,479 @@
       <c r="D1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="49" t="s">
         <v>300</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="49" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="G1" s="52" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="39" t="s">
         <v>231</v>
       </c>
       <c r="B2" s="32" t="s">
         <v>229</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="42" t="s">
         <v>259</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="44" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="39" t="s">
         <v>249</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>245</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="43" t="s">
         <v>260</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="44" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="39" t="s">
         <v>250</v>
       </c>
       <c r="B4" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="43" t="s">
         <v>260</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="44" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="40" t="s">
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="39" t="s">
         <v>171</v>
       </c>
       <c r="B5" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="43" t="s">
         <v>251</v>
       </c>
       <c r="D5" s="34" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="40" t="s">
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="39" t="s">
         <v>201</v>
       </c>
       <c r="B6" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="43" t="s">
         <v>256</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="40" t="s">
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="39" t="s">
         <v>209</v>
       </c>
       <c r="B7" s="32" t="s">
         <v>208</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="43" t="s">
         <v>255</v>
       </c>
       <c r="D7" s="34" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="40" t="s">
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="39" t="s">
         <v>233</v>
       </c>
       <c r="B8" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="43" t="s">
         <v>257</v>
       </c>
       <c r="D8" s="34" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="39" t="s">
         <v>234</v>
       </c>
       <c r="B9" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="43" t="s">
         <v>258</v>
       </c>
       <c r="D9" s="34" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="40" t="s">
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="39" t="s">
         <v>232</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>228</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="43" t="s">
         <v>259</v>
       </c>
       <c r="D10" s="34" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="14.4">
+      <c r="A11" s="39" t="s">
         <v>230</v>
       </c>
       <c r="B11" s="32" t="s">
         <v>228</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="43" t="s">
         <v>259</v>
       </c>
       <c r="D11" s="34" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="40" t="s">
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="39" t="s">
         <v>247</v>
       </c>
       <c r="B12" s="32" t="s">
         <v>244</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="43" t="s">
         <v>260</v>
       </c>
       <c r="D12" s="34" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="40" t="s">
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="39" t="s">
         <v>248</v>
       </c>
       <c r="B13" s="32" t="s">
         <v>244</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="43" t="s">
         <v>260</v>
       </c>
       <c r="D13" s="34" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="40" t="s">
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="39" t="s">
         <v>207</v>
       </c>
       <c r="B14" s="32" t="s">
         <v>205</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="43" t="s">
         <v>252</v>
       </c>
       <c r="D14" s="34" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="40" t="s">
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="39" t="s">
         <v>204</v>
       </c>
       <c r="B15" s="32" t="s">
         <v>206</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="43" t="s">
         <v>252</v>
       </c>
       <c r="D15" s="34" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="40" t="s">
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="39" t="s">
         <v>238</v>
       </c>
       <c r="B16" s="32" t="s">
         <v>237</v>
       </c>
-      <c r="C16" s="46" t="s">
+      <c r="C16" s="43" t="s">
         <v>253</v>
       </c>
       <c r="D16" s="34" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="41" t="s">
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="40" t="s">
         <v>211</v>
       </c>
       <c r="B17" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="43" t="s">
         <v>261</v>
       </c>
       <c r="D17" s="34" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="41" t="s">
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="40" t="s">
         <v>240</v>
       </c>
       <c r="B18" s="34" t="s">
         <v>239</v>
       </c>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="43" t="s">
         <v>262</v>
       </c>
       <c r="D18" s="34" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="41" t="s">
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="40" t="s">
         <v>243</v>
       </c>
       <c r="B19" s="34" t="s">
         <v>241</v>
       </c>
-      <c r="C19" s="46" t="s">
+      <c r="C19" s="43" t="s">
         <v>263</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="41" t="s">
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="40" t="s">
         <v>169</v>
       </c>
       <c r="B20" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="46" t="s">
+      <c r="C20" s="43" t="s">
         <v>254</v>
       </c>
-      <c r="D20" s="48" t="s">
+      <c r="D20" s="44" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="41" t="s">
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="40" t="s">
         <v>60</v>
       </c>
       <c r="B21" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="46" t="s">
+      <c r="C21" s="43" t="s">
         <v>198</v>
       </c>
-      <c r="D21" s="48" t="s">
+      <c r="D21" s="44" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="41" t="s">
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="40" t="s">
         <v>195</v>
       </c>
       <c r="B22" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="C22" s="46" t="s">
+      <c r="C22" s="43" t="s">
         <v>199</v>
       </c>
       <c r="D22" s="34" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="41" t="s">
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="40" t="s">
         <v>167</v>
       </c>
       <c r="B23" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="C23" s="46" t="s">
+      <c r="C23" s="43" t="s">
         <v>199</v>
       </c>
       <c r="D23" s="34" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="42" t="s">
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="40" t="s">
         <v>272</v>
       </c>
       <c r="B24" s="32" t="s">
         <v>270</v>
       </c>
-      <c r="C24" s="46" t="s">
+      <c r="C24" s="43" t="s">
         <v>271</v>
       </c>
       <c r="D24" s="34" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="42" t="s">
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="40" t="s">
         <v>265</v>
       </c>
       <c r="B25" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="C25" s="46" t="s">
+      <c r="C25" s="43" t="s">
         <v>267</v>
       </c>
       <c r="D25" s="34" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="42" t="s">
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="40" t="s">
         <v>273</v>
       </c>
       <c r="B26" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="C26" s="46" t="s">
+      <c r="C26" s="43" t="s">
         <v>269</v>
       </c>
-      <c r="D26" s="48" t="s">
+      <c r="D26" s="44" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="43" t="s">
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="40" t="s">
         <v>288</v>
       </c>
-      <c r="B27" s="44" t="s">
+      <c r="B27" s="34" t="s">
         <v>289</v>
       </c>
-      <c r="C27" s="47" t="s">
+      <c r="C27" s="43" t="s">
         <v>290</v>
       </c>
-      <c r="D27" s="44" t="s">
+      <c r="D27" s="34" t="s">
         <v>292</v>
       </c>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="43" t="s">
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="40" t="s">
         <v>293</v>
       </c>
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="34" t="s">
         <v>294</v>
       </c>
-      <c r="C28" s="47" t="s">
+      <c r="C28" s="43" t="s">
         <v>290</v>
       </c>
-      <c r="D28" s="44" t="s">
+      <c r="D28" s="34" t="s">
         <v>292</v>
       </c>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="42" t="s">
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="40" t="s">
         <v>295</v>
       </c>
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="34" t="s">
         <v>296</v>
       </c>
-      <c r="C29" s="47" t="s">
+      <c r="C29" s="43" t="s">
         <v>297</v>
       </c>
-      <c r="D29" s="44" t="s">
+      <c r="D29" s="34" t="s">
         <v>291</v>
       </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="42" t="s">
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="40" t="s">
         <v>298</v>
       </c>
-      <c r="B30" s="44" t="s">
+      <c r="B30" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="C30" s="47" t="s">
+      <c r="C30" s="43" t="s">
         <v>297</v>
       </c>
-      <c r="D30" s="44" t="s">
+      <c r="D30" s="34" t="s">
         <v>291</v>
       </c>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4093,629 +4521,182 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:D7"/>
+      <selection sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="17.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="17.21875" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="17" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>2</v>
+        <v>371</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>4</v>
+        <v>370</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.4">
+      <c r="A2" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>366</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.4">
+      <c r="A3" s="17" t="s">
+        <v>365</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>363</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.4">
       <c r="A4" s="17" t="s">
-        <v>140</v>
+        <v>362</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>65</v>
+        <v>361</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.4">
       <c r="A5" s="17" t="s">
-        <v>60</v>
+        <v>359</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>66</v>
+        <v>358</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>357</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.4">
       <c r="A6" s="17" t="s">
-        <v>141</v>
+        <v>295</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>142</v>
+        <v>356</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>355</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.4">
       <c r="A7" s="17" t="s">
-        <v>144</v>
+        <v>354</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>145</v>
+        <v>353</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="D40" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="D42" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>59</v>
+        <v>352</v>
+      </c>
+      <c r="D7" s="51" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.4">
+      <c r="A8" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.4">
+      <c r="A9" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.4">
+      <c r="A10" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>343</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.4">
+      <c r="A11" s="17" t="s">
+        <v>342</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>341</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
-      <formula1>"ASR,cBR8,uBR10K,DTI,RFGW,QB"</formula1>
+      <formula1>"ASR,cBR8,uBR10K,DTI,RFGW,QB,CGNAT"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4735,7 +4716,7 @@
       <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="17.21875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
@@ -4744,7 +4725,7 @@
     <col min="5" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -4758,7 +4739,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="14.4">
       <c r="A2" s="18" t="s">
         <v>171</v>
       </c>
@@ -4772,7 +4753,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="1" customFormat="1" ht="14.4">
       <c r="A3" s="18" t="s">
         <v>201</v>
       </c>
@@ -4786,7 +4767,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="1" customFormat="1" ht="14.4">
       <c r="A4" s="18" t="s">
         <v>209</v>
       </c>
@@ -4800,7 +4781,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="1" customFormat="1" ht="14.4">
       <c r="A5" s="19" t="s">
         <v>233</v>
       </c>
@@ -4814,7 +4795,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" s="19" t="s">
         <v>234</v>
       </c>
@@ -4828,7 +4809,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="19" t="s">
         <v>232</v>
       </c>
@@ -4842,7 +4823,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" s="19" t="s">
         <v>230</v>
       </c>
@@ -4856,7 +4837,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="19" t="s">
         <v>231</v>
       </c>
@@ -4870,7 +4851,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" s="27" t="s">
         <v>247</v>
       </c>
@@ -4884,7 +4865,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" s="27" t="s">
         <v>248</v>
       </c>
@@ -4898,7 +4879,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" s="27" t="s">
         <v>249</v>
       </c>
@@ -4912,7 +4893,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="27" t="s">
         <v>250</v>
       </c>
@@ -4926,7 +4907,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" s="18" t="s">
         <v>207</v>
       </c>
@@ -4940,7 +4921,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" s="18" t="s">
         <v>204</v>
       </c>
@@ -4954,7 +4935,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" s="19" t="s">
         <v>238</v>
       </c>
@@ -4968,7 +4949,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="17" t="s">
         <v>211</v>
       </c>
@@ -4982,7 +4963,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="22" t="s">
         <v>240</v>
       </c>
@@ -4996,7 +4977,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="28" t="s">
         <v>243</v>
       </c>
@@ -5031,10 +5012,10 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="A1:D23"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="17.21875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
@@ -5043,7 +5024,7 @@
     <col min="5" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -5057,7 +5038,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="18" t="s">
         <v>171</v>
       </c>
@@ -5071,7 +5052,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="18" t="s">
         <v>201</v>
       </c>
@@ -5085,7 +5066,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" s="18" t="s">
         <v>209</v>
       </c>
@@ -5099,7 +5080,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" s="19" t="s">
         <v>233</v>
       </c>
@@ -5113,7 +5094,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" s="19" t="s">
         <v>234</v>
       </c>
@@ -5127,7 +5108,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" s="23" customFormat="1">
       <c r="A7" s="19" t="s">
         <v>232</v>
       </c>
@@ -5141,7 +5122,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" s="24" customFormat="1" ht="14.4">
       <c r="A8" s="19" t="s">
         <v>230</v>
       </c>
@@ -5155,7 +5136,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" s="23" customFormat="1">
       <c r="A9" s="19" t="s">
         <v>231</v>
       </c>
@@ -5169,7 +5150,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" s="23" customFormat="1">
       <c r="A10" s="27" t="s">
         <v>247</v>
       </c>
@@ -5183,7 +5164,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" s="23" customFormat="1">
       <c r="A11" s="27" t="s">
         <v>248</v>
       </c>
@@ -5197,7 +5178,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" s="23" customFormat="1">
       <c r="A12" s="27" t="s">
         <v>249</v>
       </c>
@@ -5211,7 +5192,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" s="23" customFormat="1">
       <c r="A13" s="27" t="s">
         <v>250</v>
       </c>
@@ -5225,7 +5206,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" s="18" t="s">
         <v>207</v>
       </c>
@@ -5239,7 +5220,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" s="9" customFormat="1">
       <c r="A15" s="18" t="s">
         <v>204</v>
       </c>
@@ -5253,7 +5234,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" s="9" customFormat="1">
       <c r="A16" s="19" t="s">
         <v>238</v>
       </c>
@@ -5267,7 +5248,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="17" t="s">
         <v>211</v>
       </c>
@@ -5281,7 +5262,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="22" t="s">
         <v>240</v>
       </c>
@@ -5295,7 +5276,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="28" t="s">
         <v>243</v>
       </c>
@@ -5309,7 +5290,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" s="17" t="s">
         <v>169</v>
       </c>
@@ -5323,7 +5304,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4">
       <c r="A21" s="17" t="s">
         <v>60</v>
       </c>
@@ -5337,7 +5318,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" s="17" t="s">
         <v>195</v>
       </c>
@@ -5351,7 +5332,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4">
       <c r="A23" s="17" t="s">
         <v>167</v>
       </c>
@@ -5377,6 +5358,166 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:A92"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="127.44140625" style="9" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16.2">
+      <c r="A2" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="16.2">
+      <c r="A28" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="16.2">
+      <c r="A54" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="16.2">
+      <c r="A92" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:A65"/>
+  <sheetViews>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.2"/>
+  <cols>
+    <col min="1" max="1" width="101.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="11"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" location="F!H1ZWEB7T!IKRIVw3pghS-ox-w64XeCQ" display="https://mega.nz/ - F!H1ZWEB7T!IKRIVw3pghS-ox-w64XeCQ"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
@@ -5386,16 +5527,16 @@
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="89.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="96.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>332</v>
       </c>
@@ -5403,82 +5544,82 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" s="5" t="s">
         <v>46</v>
       </c>
@@ -5486,7 +5627,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" s="5" t="s">
         <v>47</v>
       </c>
@@ -5494,7 +5635,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19" s="5" t="s">
         <v>48</v>
       </c>
@@ -5502,7 +5643,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
       <c r="A20" s="5" t="s">
         <v>49</v>
       </c>
@@ -5510,52 +5651,52 @@
         <v>320</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2">
       <c r="A24" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="A25" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2">
       <c r="A27" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2">
       <c r="A29" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2">
       <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
@@ -5576,161 +5717,161 @@
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="97" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="96.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="16.2">
       <c r="A1" s="2" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1">
       <c r="A3" s="3" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1">
       <c r="A4" s="3" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1">
       <c r="A5" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1">
       <c r="A6" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1">
       <c r="A8" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1">
       <c r="A11" s="3" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1">
       <c r="A14" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1">
       <c r="A15" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1">
       <c r="A16" s="3" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1">
       <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1">
       <c r="A20" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1">
       <c r="A21" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1">
       <c r="A22" s="3" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1">
       <c r="A23" s="3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1">
       <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="17.25" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1">
       <c r="A26" s="3" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1">
       <c r="A27" s="3" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1">
       <c r="A28" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1">
       <c r="A29" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1">
       <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
@@ -5753,98 +5894,98 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="97" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="16.2">
       <c r="A1" s="2" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1">
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1">
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1">
       <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1">
       <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
@@ -5868,58 +6009,58 @@
       <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="23.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1">
       <c r="A11" s="5"/>
     </row>
   </sheetData>
@@ -5931,19 +6072,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="107.6640625" style="37" customWidth="1"/>
+    <col min="1" max="1" width="116.21875" style="37" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="8.88671875" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="16.2">
       <c r="A1" s="36" t="s">
         <v>334</v>
       </c>
@@ -5951,32 +6096,32 @@
         <v>330</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="37" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="37" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="37" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="37" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" s="37" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" s="37" t="s">
         <v>313</v>
       </c>
@@ -5984,7 +6129,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" s="37" t="s">
         <v>314</v>
       </c>
@@ -5992,7 +6137,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" s="37" t="s">
         <v>315</v>
       </c>
@@ -6000,7 +6145,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" s="37" t="s">
         <v>283</v>
       </c>
@@ -6008,7 +6153,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" s="37" t="s">
         <v>284</v>
       </c>
@@ -6016,7 +6161,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" s="37" t="s">
         <v>285</v>
       </c>
@@ -6024,7 +6169,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" s="37" t="s">
         <v>321</v>
       </c>
@@ -6032,7 +6177,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" s="37" t="s">
         <v>322</v>
       </c>
@@ -6040,7 +6185,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" s="37" t="s">
         <v>323</v>
       </c>
@@ -6048,7 +6193,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" s="37" t="s">
         <v>324</v>
       </c>
@@ -6056,7 +6201,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" s="37" t="s">
         <v>325</v>
       </c>
@@ -6064,7 +6209,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" s="37" t="s">
         <v>326</v>
       </c>
@@ -6072,12 +6217,12 @@
         <v>319</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19" s="37" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
       <c r="A20" s="37" t="s">
         <v>287</v>
       </c>
@@ -6101,113 +6246,113 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="93.109375" style="1" customWidth="1"/>
     <col min="2" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="16.2">
       <c r="A1" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+    <row r="2" spans="1:1" ht="15.6">
+      <c r="A2" s="48" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="49" t="s">
+    <row r="3" spans="1:1" ht="15.6">
+      <c r="A3" s="45" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="49" t="s">
+    <row r="4" spans="1:1" ht="15.6">
+      <c r="A4" s="45" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="49" t="s">
+    <row r="5" spans="1:1" ht="15.6">
+      <c r="A5" s="45" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50" t="s">
+    <row r="6" spans="1:1">
+      <c r="A6" s="46" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="49" t="s">
+    <row r="7" spans="1:1" ht="15.6">
+      <c r="A7" s="45" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="49" t="s">
+    <row r="8" spans="1:1" ht="15.6">
+      <c r="A8" s="45" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="49" t="s">
+    <row r="9" spans="1:1" ht="15.6">
+      <c r="A9" s="45" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="49" t="s">
+    <row r="10" spans="1:1" ht="15.6">
+      <c r="A10" s="45" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="51" t="s">
+    <row r="11" spans="1:1" ht="15.6">
+      <c r="A11" s="47" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="49" t="s">
+    <row r="12" spans="1:1" ht="15.6">
+      <c r="A12" s="45" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="15.6">
       <c r="A13" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" ht="15.6">
       <c r="A14" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" ht="15.6">
       <c r="A15" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" ht="15.6">
       <c r="A16" s="3" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="15.6">
       <c r="A17" s="5" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="15.6">
       <c r="A18" s="3" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="15.6">
       <c r="A19" s="3" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1">
       <c r="A21" s="1" t="s">
         <v>279</v>
       </c>
@@ -6222,159 +6367,948 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FF0070C0"/>
+    <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:A65"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="101.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="12" t="s">
-        <v>155</v>
+    <row r="1" spans="1:4">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" location="F!H1ZWEB7T!IKRIVw3pghS-ox-w64XeCQ" display="https://mega.nz/ - F!H1ZWEB7T!IKRIVw3pghS-ox-w64XeCQ"/>
-  </hyperlinks>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+      <formula1>"ASR,cBR8,uBR10K,DTI,RFGW,QB"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FF0070C0"/>
+    <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:A92"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="127.44140625" style="9" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="29.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="17" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="9" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A54" s="9" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="9" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A92" s="13" t="s">
-        <v>172</v>
+    <row r="1" spans="1:4">
+      <c r="A1" s="14" t="s">
+        <v>429</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.6">
+      <c r="A2" s="54" t="s">
+        <v>425</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>424</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>423</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.6">
+      <c r="A3" s="54" t="s">
+        <v>422</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>421</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>420</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6">
+      <c r="A4" s="54" t="s">
+        <v>419</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>418</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.6">
+      <c r="A5" s="54" t="s">
+        <v>416</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>415</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>414</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.6">
+      <c r="A6" s="54" t="s">
+        <v>413</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>412</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>411</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.6">
+      <c r="A7" s="54" t="s">
+        <v>410</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>408</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.6">
+      <c r="A8" s="54" t="s">
+        <v>407</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>406</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.6">
+      <c r="A9" s="54" t="s">
+        <v>405</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>404</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>403</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.6">
+      <c r="A10" s="54" t="s">
+        <v>402</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>401</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.6">
+      <c r="A11" s="54" t="s">
+        <v>399</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>398</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>397</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.6">
+      <c r="A12" s="54" t="s">
+        <v>396</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>395</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>394</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.6">
+      <c r="A13" s="53" t="s">
+        <v>265</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>392</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.6">
+      <c r="A14" s="53" t="s">
+        <v>391</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>389</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.6">
+      <c r="A15" s="53" t="s">
+        <v>388</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>387</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>386</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.6">
+      <c r="A16" s="53" t="s">
+        <v>385</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>384</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.6">
+      <c r="A17" s="53" t="s">
+        <v>383</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>382</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.6">
+      <c r="A18" s="53" t="s">
+        <v>380</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>379</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>378</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.6">
+      <c r="A19" s="53" t="s">
+        <v>377</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>376</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>375</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.6">
+      <c r="A20" s="53" t="s">
+        <v>374</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>373</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>372</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+      <formula1>"ASR,cBR8,uBR10K,DTI,RFGW,QB,CGNAT"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>